<commit_message>
add cortage to gallery images
</commit_message>
<xml_diff>
--- a/src/others/newsTable.xlsx
+++ b/src/others/newsTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\AngarPro2021\src\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\angar_pro_2021\src\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Склад расположен на территории завода и предназначен для готовой продукции не требующей теплого помещения для хранения.</t>
+  </si>
+  <si>
+    <t>/img/photos/gallery/015__001-photo-</t>
+  </si>
+  <si>
+    <t>/img/photos/gallery/014__013-photo-</t>
+  </si>
+  <si>
+    <t>Завершили строительство КСК</t>
+  </si>
+  <si>
+    <t>Конно-спортивный комплекс в деревне Онуфриево, Москоской области. На этот год все. Манеж закончили. В 2021 году конюшни и прочая инфраструктура.</t>
   </si>
 </sst>
 </file>
@@ -479,23 +491,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
+    <col min="2" max="2" width="33.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -515,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -523,7 +535,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="8">
-        <f t="shared" ref="C2:C12" si="0">D2</f>
+        <f t="shared" ref="C2:C13" si="0">D2</f>
         <v>43276</v>
       </c>
       <c r="D2" s="2">
@@ -536,7 +548,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -557,7 +569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -578,7 +590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -599,7 +611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -620,7 +632,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -641,7 +653,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -662,7 +674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -683,7 +695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -704,7 +716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -725,10 +737,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="8">
         <f t="shared" si="0"/>
         <v>44211</v>
@@ -741,6 +756,27 @@
       </c>
       <c r="F12" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="0"/>
+        <v>44193</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44193</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>